<commit_message>
Update base-version-schedule in docs
</commit_message>
<xml_diff>
--- a/docs/marzec_2021_wersja_bazowa.xlsx
+++ b/docs/marzec_2021_wersja_bazowa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="95">
   <si>
     <t xml:space="preserve">GRAFIK |  MIESIĄC MARZEC  |  ROK 2021  |  LICZBA GODZ 184</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pracownik 25</t>
   </si>
   <si>
     <t xml:space="preserve">Nazwa zmiany</t>
@@ -776,7 +773,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="2" style="0" width="4.38"/>
@@ -6032,7 +6029,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6045,13 +6042,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN1000"/>
+  <dimension ref="A1:AN1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="K31" activeCellId="0" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.27"/>
@@ -6564,21 +6561,11 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
@@ -13384,17 +13371,11 @@
       <c r="D999" s="2"/>
       <c r="E999" s="2"/>
     </row>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -13413,7 +13394,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -13425,22 +13406,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -13521,10 +13502,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>13</v>
@@ -13533,13 +13514,13 @@
         <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -13551,16 +13532,16 @@
         <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>7</v>
@@ -13569,16 +13550,16 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>23</v>
@@ -13587,16 +13568,16 @@
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>7</v>
@@ -13605,16 +13586,16 @@
         <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>7</v>
@@ -13623,13 +13604,13 @@
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
@@ -13641,16 +13622,16 @@
         <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>7</v>
@@ -13659,13 +13640,13 @@
         <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -13677,13 +13658,13 @@
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>49</v>
@@ -13695,13 +13676,13 @@
         <v>19</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="20"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -13713,13 +13694,13 @@
         <v>19</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>10</v>
@@ -13731,13 +13712,13 @@
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
@@ -13749,13 +13730,13 @@
         <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>23</v>
@@ -13767,16 +13748,16 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
@@ -13785,13 +13766,13 @@
         <v>24</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>13</v>
@@ -13803,16 +13784,16 @@
         <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>0</v>
@@ -13821,16 +13802,16 @@
         <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>0</v>
@@ -13839,16 +13820,16 @@
         <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
@@ -13857,16 +13838,16 @@
         <v>24</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
@@ -13875,16 +13856,16 @@
         <v>24</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>0</v>
@@ -13893,16 +13874,16 @@
         <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
@@ -13911,16 +13892,16 @@
         <v>24</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>0</v>
@@ -13929,7 +13910,7 @@
         <v>24</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" s="27"/>
     </row>
@@ -21736,7 +21717,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Change function names and moves 7 to const
</commit_message>
<xml_diff>
--- a/docs/marzec_2021_wersja_bazowa.xlsx
+++ b/docs/marzec_2021_wersja_bazowa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="grafik" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="97">
   <si>
     <t xml:space="preserve">GRAFIK |  MIESIĄC MARZEC  |  ROK 2021  |  LICZBA GODZ 184</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">NIE</t>
@@ -776,7 +779,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="2" style="0" width="4.38"/>
@@ -6047,11 +6050,11 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.27"/>
@@ -13409,11 +13412,11 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -13778,158 +13781,158 @@
       <c r="B17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>24</v>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>24</v>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>24</v>
+        <v>84</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>24</v>
+        <v>86</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>24</v>
+        <v>88</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>24</v>
+        <v>90</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>24</v>
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>24</v>
+        <v>94</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F25" s="27"/>
     </row>

</xml_diff>

<commit_message>
TASK-418 Disallow working shifts that cross 7am  (#341)
* add check

* handle non working shifts

* Change function names and moves 7 to const

Co-authored-by: Bohdan Forostianyi <qwebeck5@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/marzec_2021_wersja_bazowa.xlsx
+++ b/docs/marzec_2021_wersja_bazowa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="grafik" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="97">
   <si>
     <t xml:space="preserve">GRAFIK |  MIESIĄC MARZEC  |  ROK 2021  |  LICZBA GODZ 184</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">NIE</t>
@@ -776,7 +779,7 @@
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="2" style="0" width="4.38"/>
@@ -6047,11 +6050,11 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.27"/>
@@ -13409,11 +13412,11 @@
   </sheetPr>
   <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.87"/>
@@ -13778,158 +13781,158 @@
       <c r="B17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>24</v>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>24</v>
+      <c r="C18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>24</v>
+        <v>84</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>24</v>
+        <v>86</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>24</v>
+        <v>88</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>24</v>
+        <v>90</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>24</v>
+        <v>92</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>24</v>
+        <v>94</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F25" s="27"/>
     </row>

</xml_diff>